<commit_message>
create rows with list
</commit_message>
<xml_diff>
--- a/hope/GeneratedExcel.xlsx
+++ b/hope/GeneratedExcel.xlsx
@@ -12,18 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>cell0</t>
+    <t>data0</t>
   </si>
   <si>
-    <t>cell2</t>
-  </si>
-  <si>
-    <t>cell in row2</t>
-  </si>
-  <si>
-    <t>row3</t>
+    <t>data1</t>
   </si>
 </sst>
 </file>
@@ -68,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -78,18 +72,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>